<commit_message>
Update event message in main.py for upcoming gathering on May 4th
</commit_message>
<xml_diff>
--- a/LISTE AFE OK.xlsx
+++ b/LISTE AFE OK.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="414">
   <si>
     <t>NOM</t>
   </si>
@@ -223,42 +223,6 @@
     <t>2250759710846</t>
   </si>
   <si>
-    <t>NADEGE</t>
-  </si>
-  <si>
-    <t>2250757090663</t>
-  </si>
-  <si>
-    <t>MON PÈRE</t>
-  </si>
-  <si>
-    <t>2250707610265</t>
-  </si>
-  <si>
-    <t>MAMAN NADEGE</t>
-  </si>
-  <si>
-    <t>2250778691485</t>
-  </si>
-  <si>
-    <t>GASTON</t>
-  </si>
-  <si>
-    <t>2250758656560</t>
-  </si>
-  <si>
-    <t>MARIE PAULE</t>
-  </si>
-  <si>
-    <t>2250758744596</t>
-  </si>
-  <si>
-    <t>ARISTINE</t>
-  </si>
-  <si>
-    <t>2250749705334</t>
-  </si>
-  <si>
     <t>SIO ROSE</t>
   </si>
   <si>
@@ -445,12 +409,6 @@
     <t>2250787233748</t>
   </si>
   <si>
-    <t>B Jean Francois</t>
-  </si>
-  <si>
-    <t>2250709122448</t>
-  </si>
-  <si>
     <t>Bienvenu</t>
   </si>
   <si>
@@ -1225,18 +1183,6 @@
     <t>2250779351060</t>
   </si>
   <si>
-    <t>Berger Gerard</t>
-  </si>
-  <si>
-    <t>2250749273342</t>
-  </si>
-  <si>
-    <t>Cédric DUAKON</t>
-  </si>
-  <si>
-    <t>2250788466748</t>
-  </si>
-  <si>
     <t>EBY ADJO JOSIANE</t>
   </si>
   <si>
@@ -1295,6 +1241,12 @@
   </si>
   <si>
     <t>2250707618381</t>
+  </si>
+  <si>
+    <t>KOUASSI BERTRAND</t>
+  </si>
+  <si>
+    <t>2250759781957</t>
   </si>
   <si>
     <t>CADIO SHERYDAN</t>
@@ -1307,7 +1259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1323,11 +1275,6 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1370,7 +1317,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1381,8 +1328,7 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1939,30 +1885,6 @@
       <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-      <c r="Z41" s="4"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
@@ -2206,63 +2128,63 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>156</v>
@@ -2334,399 +2256,399 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="2" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="2" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="2" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>185</v>
+        <v>228</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>229</v>
@@ -2766,63 +2688,63 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B142" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B145" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B146" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B147" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B148" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>44</v>
+        <v>251</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>252</v>
@@ -2910,119 +2832,119 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B161" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B162" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B163" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B165" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B166" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>26</v>
+        <v>249</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B169" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B170" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B171" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B172" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B173" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="2" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>300</v>
@@ -3118,63 +3040,63 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B189" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B190" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B191" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="2" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>337</v>
@@ -3389,902 +3311,846 @@
       </c>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="2" t="s">
+      <c r="A220" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B220" s="3" t="s">
+      <c r="B220" s="5" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="2" t="s">
+      <c r="A221" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B221" s="3" t="s">
+      <c r="B221" s="5" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="2" t="s">
+      <c r="A222" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="B222" s="3" t="s">
+      <c r="B222" s="5" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B223" s="3" t="s">
+      <c r="B223" s="5" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="2" t="s">
+      <c r="A224" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="B224" s="3" t="s">
+      <c r="B224" s="5" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="2" t="s">
+      <c r="A225" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B225" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B225" s="3" t="s">
+    </row>
+    <row r="226" ht="15.75" customHeight="1">
+      <c r="A226" s="4" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="2" t="s">
+      <c r="B226" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="B226" s="3" t="s">
+    </row>
+    <row r="227" ht="15.75" customHeight="1">
+      <c r="A227" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="2" t="s">
+      <c r="B227" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="B227" s="3" t="s">
+    </row>
+    <row r="228" ht="15.75" customHeight="1">
+      <c r="A228" s="4" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="2" t="s">
+      <c r="B228" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="B228" s="3" t="s">
+    </row>
+    <row r="229" ht="15.75" customHeight="1">
+      <c r="A229" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B229" s="5" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="5" t="s">
+    <row r="230" ht="15.75" customHeight="1">
+      <c r="A230" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="B229" s="6" t="s">
+      <c r="B230" s="5" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="5" t="s">
+    <row r="231" ht="15.75" customHeight="1">
+      <c r="A231" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="B230" s="6" t="s">
+      <c r="B231" s="5" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="5" t="s">
+    <row r="232" ht="15.75" customHeight="1">
+      <c r="A232" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="B231" s="6" t="s">
+      <c r="B232" s="5" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B233" s="6" t="s">
-        <v>417</v>
-      </c>
+      <c r="B233" s="6"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B234" s="6" t="s">
-        <v>418</v>
-      </c>
+      <c r="B234" s="6"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B235" s="6" t="s">
-        <v>420</v>
-      </c>
+      <c r="B235" s="6"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B236" s="6" t="s">
-        <v>422</v>
-      </c>
+      <c r="B236" s="6"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B237" s="6" t="s">
-        <v>424</v>
-      </c>
+      <c r="B237" s="6"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>425</v>
-      </c>
+      <c r="B238" s="6"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B239" s="6" t="s">
-        <v>427</v>
-      </c>
+      <c r="B239" s="6"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B240" s="6" t="s">
-        <v>429</v>
-      </c>
+      <c r="B240" s="6"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="B241" s="7"/>
+      <c r="B241" s="6"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="B242" s="7"/>
+      <c r="B242" s="6"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="B243" s="7"/>
+      <c r="B243" s="6"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="B244" s="7"/>
+      <c r="B244" s="6"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="B245" s="7"/>
+      <c r="B245" s="6"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="B246" s="7"/>
+      <c r="B246" s="6"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="B247" s="7"/>
+      <c r="B247" s="6"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="B248" s="7"/>
+      <c r="B248" s="6"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="B249" s="7"/>
+      <c r="B249" s="6"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="B250" s="7"/>
+      <c r="B250" s="6"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="B251" s="7"/>
+      <c r="B251" s="6"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="B252" s="7"/>
+      <c r="B252" s="6"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="B253" s="7"/>
+      <c r="B253" s="6"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="B254" s="7"/>
+      <c r="B254" s="6"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="B255" s="7"/>
+      <c r="B255" s="6"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="B256" s="7"/>
+      <c r="B256" s="6"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="B257" s="7"/>
+      <c r="B257" s="6"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="B258" s="7"/>
+      <c r="B258" s="6"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="7"/>
+      <c r="B259" s="6"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="B260" s="7"/>
+      <c r="B260" s="6"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="B261" s="7"/>
+      <c r="B261" s="6"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="B262" s="7"/>
+      <c r="B262" s="6"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="B263" s="7"/>
+      <c r="B263" s="6"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="B264" s="7"/>
+      <c r="B264" s="6"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="B265" s="7"/>
+      <c r="B265" s="6"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="B266" s="7"/>
+      <c r="B266" s="6"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="B267" s="7"/>
+      <c r="B267" s="6"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="B268" s="7"/>
+      <c r="B268" s="6"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="B269" s="7"/>
+      <c r="B269" s="6"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="B270" s="7"/>
+      <c r="B270" s="6"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="B271" s="7"/>
+      <c r="B271" s="6"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="B272" s="7"/>
+      <c r="B272" s="6"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="B273" s="7"/>
+      <c r="B273" s="6"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="B274" s="7"/>
+      <c r="B274" s="6"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="B275" s="7"/>
+      <c r="B275" s="6"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="B276" s="7"/>
+      <c r="B276" s="6"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="B277" s="7"/>
+      <c r="B277" s="6"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="B278" s="7"/>
+      <c r="B278" s="6"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="B279" s="7"/>
+      <c r="B279" s="6"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="B280" s="7"/>
+      <c r="B280" s="6"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="B281" s="7"/>
+      <c r="B281" s="6"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="B282" s="7"/>
+      <c r="B282" s="6"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="B283" s="7"/>
+      <c r="B283" s="6"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="B284" s="7"/>
+      <c r="B284" s="6"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="B285" s="7"/>
+      <c r="B285" s="6"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="B286" s="7"/>
+      <c r="B286" s="6"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="B287" s="7"/>
+      <c r="B287" s="6"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="B288" s="7"/>
+      <c r="B288" s="6"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="B289" s="7"/>
+      <c r="B289" s="6"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="B290" s="7"/>
+      <c r="B290" s="6"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="B291" s="7"/>
+      <c r="B291" s="6"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="B292" s="7"/>
+      <c r="B292" s="6"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="B293" s="7"/>
+      <c r="B293" s="6"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="B294" s="7"/>
+      <c r="B294" s="6"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="B295" s="7"/>
+      <c r="B295" s="6"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="B296" s="7"/>
+      <c r="B296" s="6"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="B297" s="7"/>
+      <c r="B297" s="6"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="B298" s="7"/>
+      <c r="B298" s="6"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="B299" s="7"/>
+      <c r="B299" s="6"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="B300" s="7"/>
+      <c r="B300" s="6"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="B301" s="7"/>
+      <c r="B301" s="6"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="B302" s="7"/>
+      <c r="B302" s="6"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="B303" s="7"/>
+      <c r="B303" s="6"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="B304" s="7"/>
+      <c r="B304" s="6"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="B305" s="7"/>
+      <c r="B305" s="6"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="B306" s="7"/>
+      <c r="B306" s="6"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="B307" s="7"/>
+      <c r="B307" s="6"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="B308" s="7"/>
+      <c r="B308" s="6"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="B309" s="7"/>
+      <c r="B309" s="6"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="B310" s="7"/>
+      <c r="B310" s="6"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="B311" s="7"/>
+      <c r="B311" s="6"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="B312" s="7"/>
+      <c r="B312" s="6"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="B313" s="7"/>
+      <c r="B313" s="6"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="B314" s="7"/>
+      <c r="B314" s="6"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="B315" s="7"/>
+      <c r="B315" s="6"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="B316" s="7"/>
+      <c r="B316" s="6"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="B317" s="7"/>
+      <c r="B317" s="6"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="B318" s="7"/>
+      <c r="B318" s="6"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="B319" s="7"/>
+      <c r="B319" s="6"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="B320" s="7"/>
+      <c r="B320" s="6"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="B321" s="7"/>
+      <c r="B321" s="6"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="B322" s="7"/>
+      <c r="B322" s="6"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="B323" s="7"/>
+      <c r="B323" s="6"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="B324" s="7"/>
+      <c r="B324" s="6"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="B325" s="7"/>
+      <c r="B325" s="6"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="B326" s="7"/>
+      <c r="B326" s="6"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="B327" s="7"/>
+      <c r="B327" s="6"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="B328" s="7"/>
+      <c r="B328" s="6"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="B329" s="7"/>
+      <c r="B329" s="6"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="B330" s="7"/>
+      <c r="B330" s="6"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="B331" s="7"/>
+      <c r="B331" s="6"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="B332" s="7"/>
+      <c r="B332" s="6"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="B333" s="7"/>
+      <c r="B333" s="6"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="B334" s="7"/>
+      <c r="B334" s="6"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="B335" s="7"/>
+      <c r="B335" s="6"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="B336" s="7"/>
+      <c r="B336" s="6"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="B337" s="7"/>
+      <c r="B337" s="6"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="B338" s="7"/>
+      <c r="B338" s="6"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="B339" s="7"/>
+      <c r="B339" s="6"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="B340" s="7"/>
+      <c r="B340" s="6"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="B341" s="7"/>
+      <c r="B341" s="6"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="B342" s="7"/>
+      <c r="B342" s="6"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="B343" s="7"/>
+      <c r="B343" s="6"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="B344" s="7"/>
+      <c r="B344" s="6"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="B345" s="7"/>
+      <c r="B345" s="6"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="B346" s="7"/>
+      <c r="B346" s="6"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="B347" s="7"/>
+      <c r="B347" s="6"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="B348" s="7"/>
+      <c r="B348" s="6"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="B349" s="7"/>
+      <c r="B349" s="6"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="B350" s="7"/>
+      <c r="B350" s="6"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="B351" s="7"/>
+      <c r="B351" s="6"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="B352" s="7"/>
+      <c r="B352" s="6"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="B353" s="7"/>
+      <c r="B353" s="6"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="B354" s="7"/>
+      <c r="B354" s="6"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="B355" s="7"/>
+      <c r="B355" s="6"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="B356" s="7"/>
+      <c r="B356" s="6"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="B357" s="7"/>
+      <c r="B357" s="6"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="B358" s="7"/>
+      <c r="B358" s="6"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="B359" s="7"/>
+      <c r="B359" s="6"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="B360" s="7"/>
+      <c r="B360" s="6"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="B361" s="7"/>
+      <c r="B361" s="6"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="B362" s="7"/>
+      <c r="B362" s="6"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="B363" s="7"/>
+      <c r="B363" s="6"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="B364" s="7"/>
+      <c r="B364" s="6"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="B365" s="7"/>
+      <c r="B365" s="6"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="B366" s="7"/>
+      <c r="B366" s="6"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="B367" s="7"/>
+      <c r="B367" s="6"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="B368" s="7"/>
+      <c r="B368" s="6"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="B369" s="7"/>
+      <c r="B369" s="6"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="B370" s="7"/>
+      <c r="B370" s="6"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="B371" s="7"/>
+      <c r="B371" s="6"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="B372" s="7"/>
+      <c r="B372" s="6"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="B373" s="7"/>
+      <c r="B373" s="6"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="B374" s="7"/>
+      <c r="B374" s="6"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="B375" s="7"/>
+      <c r="B375" s="6"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="B376" s="7"/>
+      <c r="B376" s="6"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="B377" s="7"/>
+      <c r="B377" s="6"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="B378" s="7"/>
+      <c r="B378" s="6"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="7"/>
+      <c r="B379" s="6"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="B380" s="7"/>
+      <c r="B380" s="6"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="B381" s="7"/>
+      <c r="B381" s="6"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="B382" s="7"/>
+      <c r="B382" s="6"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="B383" s="7"/>
+      <c r="B383" s="6"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="B384" s="7"/>
+      <c r="B384" s="6"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="B385" s="7"/>
+      <c r="B385" s="6"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="B386" s="7"/>
+      <c r="B386" s="6"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="B387" s="7"/>
+      <c r="B387" s="6"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="B388" s="7"/>
+      <c r="B388" s="6"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="B389" s="7"/>
+      <c r="B389" s="6"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="7"/>
+      <c r="B390" s="6"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="B391" s="7"/>
+      <c r="B391" s="6"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="B392" s="7"/>
+      <c r="B392" s="6"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="B393" s="7"/>
+      <c r="B393" s="6"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="B394" s="7"/>
+      <c r="B394" s="6"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="B395" s="7"/>
+      <c r="B395" s="6"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="B396" s="7"/>
+      <c r="B396" s="6"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="B397" s="7"/>
+      <c r="B397" s="6"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="B398" s="7"/>
+      <c r="B398" s="6"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="B399" s="7"/>
+      <c r="B399" s="6"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="B400" s="7"/>
+      <c r="B400" s="6"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="B401" s="7"/>
+      <c r="B401" s="6"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="B402" s="7"/>
+      <c r="B402" s="6"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="B403" s="7"/>
+      <c r="B403" s="6"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="B404" s="7"/>
+      <c r="B404" s="6"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="B405" s="7"/>
+      <c r="B405" s="6"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="B406" s="7"/>
+      <c r="B406" s="6"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="B407" s="7"/>
+      <c r="B407" s="6"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="B408" s="7"/>
+      <c r="B408" s="6"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="B409" s="7"/>
+      <c r="B409" s="6"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="B410" s="7"/>
+      <c r="B410" s="6"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="B411" s="7"/>
+      <c r="B411" s="6"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="B412" s="7"/>
+      <c r="B412" s="6"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="B413" s="7"/>
+      <c r="B413" s="6"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="B414" s="7"/>
+      <c r="B414" s="6"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="B415" s="7"/>
+      <c r="B415" s="6"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="B416" s="7"/>
+      <c r="B416" s="6"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="B417" s="7"/>
+      <c r="B417" s="6"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="B418" s="7"/>
+      <c r="B418" s="6"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="B419" s="7"/>
+      <c r="B419" s="6"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="B420" s="7"/>
+      <c r="B420" s="6"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="B421" s="7"/>
+      <c r="B421" s="6"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="B422" s="7"/>
+      <c r="B422" s="6"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="B423" s="7"/>
+      <c r="B423" s="6"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="B424" s="7"/>
+      <c r="B424" s="6"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="B425" s="7"/>
+      <c r="B425" s="6"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="B426" s="7"/>
+      <c r="B426" s="6"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="B427" s="7"/>
+      <c r="B427" s="6"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="B428" s="7"/>
+      <c r="B428" s="6"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="B429" s="7"/>
+      <c r="B429" s="6"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="B430" s="7"/>
+      <c r="B430" s="6"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="B431" s="7"/>
+      <c r="B431" s="6"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="B432" s="7"/>
+      <c r="B432" s="6"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="B433" s="7"/>
+      <c r="B433" s="6"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="B434" s="7"/>
+      <c r="B434" s="6"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="B435" s="7"/>
+      <c r="B435" s="6"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="B436" s="7"/>
+      <c r="B436" s="6"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="B437" s="7"/>
+      <c r="B437" s="6"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="B438" s="7"/>
+      <c r="B438" s="6"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="B439" s="7"/>
+      <c r="B439" s="6"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="7"/>
+      <c r="B440" s="6"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="B441" s="7"/>
+      <c r="B441" s="6"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="B442" s="7"/>
+      <c r="B442" s="6"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="B443" s="7"/>
+      <c r="B443" s="6"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="B444" s="7"/>
+      <c r="B444" s="6"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="B445" s="7"/>
+      <c r="B445" s="6"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="B446" s="7"/>
+      <c r="B446" s="6"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="B447" s="7"/>
+      <c r="B447" s="6"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="B448" s="7"/>
+      <c r="B448" s="6"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="B449" s="7"/>
+      <c r="B449" s="6"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="B450" s="7"/>
+      <c r="B450" s="6"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="B451" s="7"/>
+      <c r="B451" s="6"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="B452" s="7"/>
+      <c r="B452" s="6"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="B453" s="7"/>
+      <c r="B453" s="6"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="B454" s="7"/>
+      <c r="B454" s="6"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="B455" s="7"/>
+      <c r="B455" s="6"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="B456" s="7"/>
+      <c r="B456" s="6"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="B457" s="7"/>
+      <c r="B457" s="6"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="B458" s="7"/>
+      <c r="B458" s="6"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="B459" s="7"/>
+      <c r="B459" s="6"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="B460" s="7"/>
+      <c r="B460" s="6"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="B461" s="7"/>
+      <c r="B461" s="6"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="B462" s="7"/>
+      <c r="B462" s="6"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="B463" s="7"/>
+      <c r="B463" s="6"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="B464" s="7"/>
+      <c r="B464" s="6"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="B465" s="7"/>
+      <c r="B465" s="6"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="B466" s="7"/>
+      <c r="B466" s="6"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="B467" s="7"/>
+      <c r="B467" s="6"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="B468" s="7"/>
+      <c r="B468" s="6"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="B469" s="7"/>
+      <c r="B469" s="6"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="B470" s="7"/>
+      <c r="B470" s="6"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="B471" s="7"/>
+      <c r="B471" s="6"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="B472" s="7"/>
+      <c r="B472" s="6"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="B473" s="7"/>
+      <c r="B473" s="6"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="B474" s="7"/>
+      <c r="B474" s="6"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="B475" s="7"/>
-    </row>
-    <row r="476" ht="15.75" customHeight="1">
-      <c r="B476" s="7"/>
-    </row>
-    <row r="477" ht="15.75" customHeight="1">
-      <c r="B477" s="7"/>
-    </row>
-    <row r="478" ht="15.75" customHeight="1">
-      <c r="B478" s="7"/>
-    </row>
-    <row r="479" ht="15.75" customHeight="1">
-      <c r="B479" s="7"/>
-    </row>
-    <row r="480" ht="15.75" customHeight="1">
-      <c r="B480" s="7"/>
-    </row>
-    <row r="481" ht="15.75" customHeight="1">
-      <c r="B481" s="7"/>
-    </row>
-    <row r="482" ht="15.75" customHeight="1">
-      <c r="B482" s="7"/>
-    </row>
-    <row r="483" ht="15.75" customHeight="1">
-      <c r="B483" s="7"/>
-    </row>
+      <c r="B475" s="6"/>
+    </row>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
     <row r="484" ht="15.75" customHeight="1"/>
     <row r="485" ht="15.75" customHeight="1"/>
     <row r="486" ht="15.75" customHeight="1"/>
@@ -4794,14 +4660,6 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>